<commit_message>
Renamed appModule to WebModule
Added new scripts
Exchange_3_Appointment_Details_Page_Abort_No_Access_Chrome
Exchange_3_Appointment_Details_Page_Abort_No_Access_IE

Added test data for the 2 new scripts

Added new Methods_Appointment_Details

Updated Utils, Constant, Objects_Appointment_Details_Page,
Objects_Doorstop_Protocol_Page
</commit_message>
<xml_diff>
--- a/src/testData/Exchange_3_Return_To_Appointments_List_Page_From_Appointment_Details_Page_IE.xlsx
+++ b/src/testData/Exchange_3_Return_To_Appointments_List_Page_From_Appointment_Details_Page_IE.xlsx
@@ -30,13 +30,13 @@
     <t>User</t>
   </si>
   <si>
-    <t>Exchange_3_End_To_End_Chrome</t>
-  </si>
-  <si>
-    <t>Chrome</t>
-  </si>
-  <si>
     <t>Automation</t>
+  </si>
+  <si>
+    <t>IE</t>
+  </si>
+  <si>
+    <t>Exchange_3_Return_To_Appointments_List_Page_From_Appointment_Details_Page_IE</t>
   </si>
 </sst>
 </file>
@@ -374,7 +374,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -385,12 +385,12 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:U1048576"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="41.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="73.6640625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="7.77734375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.5546875" bestFit="1" customWidth="1" collapsed="1"/>
@@ -425,13 +425,13 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B2" t="s">
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>